<commit_message>
ホワイトボード→チラシ配布資料 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/已完成/test_ホワイトボート_トラブル一覧_new.xlsx
+++ b/test_物件管理/已完成/test_ホワイトボート_トラブル一覧_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="792" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="792" firstSheet="1" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -21,14 +21,13 @@
     <sheet name="IN_FORM_006" sheetId="23" r:id="rId12"/>
     <sheet name="EXPECT_006" sheetId="24" r:id="rId13"/>
     <sheet name="テストケース" sheetId="3" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="26" r:id="rId15"/>
   </sheets>
   <calcPr calcId="125725" calcMode="manual" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3443" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3416" uniqueCount="641">
   <si>
     <t>URL:</t>
   </si>
@@ -2349,18 +2348,6 @@
   </si>
   <si>
     <t>PAGEUP</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>URL:</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>/contract/subscription/2/change/</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAGEDOWN</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -17353,8 +17340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -17606,12 +17593,6 @@
       <c r="J14" s="63"/>
       <c r="K14" s="63"/>
       <c r="L14" s="63"/>
-      <c r="M14" s="68" t="s">
-        <v>367</v>
-      </c>
-      <c r="N14" s="68" t="s">
-        <v>230</v>
-      </c>
       <c r="Q14" s="63"/>
     </row>
     <row r="15" spans="1:17" s="68" customFormat="1">
@@ -17636,15 +17617,6 @@
       <c r="E16" s="182"/>
       <c r="F16" s="182"/>
       <c r="I16" s="63"/>
-      <c r="N16" s="68" t="s">
-        <v>435</v>
-      </c>
-      <c r="O16" s="68" t="s">
-        <v>349</v>
-      </c>
-      <c r="P16" s="68" t="s">
-        <v>350</v>
-      </c>
       <c r="Q16" s="63"/>
     </row>
     <row r="17" spans="1:17" s="68" customFormat="1">
@@ -17663,15 +17635,6 @@
         <v>588</v>
       </c>
       <c r="I17" s="63"/>
-      <c r="N17" s="68" t="s">
-        <v>438</v>
-      </c>
-      <c r="O17" s="68" t="s">
-        <v>359</v>
-      </c>
-      <c r="P17" s="68" t="s">
-        <v>360</v>
-      </c>
       <c r="Q17" s="63"/>
     </row>
     <row r="18" spans="1:17" s="68" customFormat="1">
@@ -17690,15 +17653,9 @@
       <c r="K19" s="63"/>
       <c r="L19" s="63"/>
       <c r="M19" s="68"/>
-      <c r="N19" s="68" t="s">
-        <v>467</v>
-      </c>
-      <c r="O19" s="68" t="s">
-        <v>468</v>
-      </c>
-      <c r="P19" s="68" t="s">
-        <v>469</v>
-      </c>
+      <c r="N19" s="68"/>
+      <c r="O19" s="68"/>
+      <c r="P19" s="68"/>
       <c r="Q19" s="63"/>
     </row>
     <row r="20" spans="1:17">
@@ -17740,15 +17697,9 @@
       <c r="K23" s="63"/>
       <c r="L23" s="63"/>
       <c r="M23" s="68"/>
-      <c r="N23" s="182" t="s">
-        <v>636</v>
-      </c>
-      <c r="O23" s="68" t="s">
-        <v>525</v>
-      </c>
-      <c r="P23" s="68" t="s">
-        <v>526</v>
-      </c>
+      <c r="N23" s="182"/>
+      <c r="O23" s="68"/>
+      <c r="P23" s="68"/>
       <c r="Q23" s="63"/>
     </row>
     <row r="24" spans="1:17">
@@ -17779,15 +17730,9 @@
       <c r="K26" s="63"/>
       <c r="L26" s="63"/>
       <c r="M26" s="182"/>
-      <c r="N26" s="182" t="s">
-        <v>586</v>
-      </c>
-      <c r="O26" s="182" t="s">
-        <v>587</v>
-      </c>
-      <c r="P26" s="182" t="s">
-        <v>588</v>
-      </c>
+      <c r="N26" s="182"/>
+      <c r="O26" s="182"/>
+      <c r="P26" s="182"/>
       <c r="Q26" s="63"/>
     </row>
     <row r="27" spans="1:17">
@@ -17898,71 +17843,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="195" t="s">
-        <v>641</v>
-      </c>
-      <c r="B1" s="195" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="195" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="195" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="195" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="195" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="195" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="195" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="195" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="195" t="s">
-        <v>640</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -18155,7 +18035,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>